<commit_message>
add a print to identify the forecast has started
</commit_message>
<xml_diff>
--- a/dataset/cpu.xlsx
+++ b/dataset/cpu.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B269"/>
+  <dimension ref="A1:B271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3115,6 +3115,26 @@
         <v>0.3333</v>
       </c>
     </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>04/27/2021 19:01:43</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>0.1639</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>04/27/2021 19:03:50</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>0.339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
add one folder ofr each microservice
</commit_message>
<xml_diff>
--- a/dataset/cpu.xlsx
+++ b/dataset/cpu.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,161 +438,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>05/13/2021 01:49:48</t>
+          <t>05/13/2021 20:18:13</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3333</v>
+        <v>0.3390000000000001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>05/13/2021 01:50:51</t>
+          <t>05/13/2021 20:23:32</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4126000000000001</v>
+        <v>0.3279</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>05/13/2021 01:51:53</t>
+          <t>05/13/2021 20:23:51</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4154</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>05/13/2021 01:52:55</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>05/13/2021 01:53:58</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.3334</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>05/13/2021 01:55:02</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.3333</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>05/13/2021 01:56:06</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.3279</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>05/13/2021 01:57:10</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>05/13/2021 01:58:14</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.3333</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>05/13/2021 01:59:16</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0.3279</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>05/13/2021 02:00:19</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.3390000000000001</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>05/13/2021 02:01:23</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>21.6667</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>05/13/2021 02:02:28</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>48.5</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>05/13/2021 02:03:33</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>44.3333</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>05/13/2021 02:04:39</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>41.5</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>05/13/2021 02:05:43</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>36.9054</v>
+        <v>3.500999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>